<commit_message>
refactor: Standardize on TestNG Reporter logging
- Removed Logback dependencies and configuration from project
- Implemented consistent TestNG Reporter logging across all tests
- Added detailed step-by-step action reporting for better traceability
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/login_data.xlsx
+++ b/src/test/resources/testData/login_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DEPI\Project\Automation_Exercise\src\test\resources\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03A5CCF7-8F98-4A4D-87C7-2A96507C20B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{016ACA1E-EBB0-469F-A9BC-B89F0E78DAB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{985B74B3-7B1C-4AC1-85EF-FEA90879A07F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
   <si>
     <t>id</t>
   </si>
@@ -66,6 +66,15 @@
   </si>
   <si>
     <t>wrong</t>
+  </si>
+  <si>
+    <t>hello@yahoo.com</t>
+  </si>
+  <si>
+    <t>qew2</t>
+  </si>
+  <si>
+    <t>TRUE</t>
   </si>
 </sst>
 </file>
@@ -449,10 +458,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA00FF79-CB98-4AA4-AB37-FDF7F22C9868}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="A1:XFD1048576"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -506,10 +515,25 @@
         <v>0</v>
       </c>
     </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{9E3D90B1-78CE-48FB-A54B-A059FBCB7274}"/>
     <hyperlink ref="B3" r:id="rId2" xr:uid="{2243D263-C69B-41E6-86E7-4672D72FA46E}"/>
+    <hyperlink ref="B4" r:id="rId3" xr:uid="{36C4A703-BC5D-420C-A032-1E3466CEC0CA}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>